<commit_message>
removed excel file i18n
</commit_message>
<xml_diff>
--- a/molgenis-bootstrap/src/main/resources/i18n.xlsx
+++ b/molgenis-bootstrap/src/main/resources/i18n.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="i18nstrings" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>msgid</t>
   </si>
@@ -238,42 +238,6 @@
   </si>
   <si>
     <t>Number</t>
-  </si>
-  <si>
-    <t>dataexplorer_directory_export_button</t>
-  </si>
-  <si>
-    <t>Go to sample / data negotiation</t>
-  </si>
-  <si>
-    <t>dataexplorer_directory_export_dialog_yes</t>
-  </si>
-  <si>
-    <t>Yes, Send to Negotiator</t>
-  </si>
-  <si>
-    <t>No, I want to keep filtering</t>
-  </si>
-  <si>
-    <t>dataexplorer_directory_export_dialog_no</t>
-  </si>
-  <si>
-    <t>dataexplorer_directory_export_dialog_title</t>
-  </si>
-  <si>
-    <t>Send request to the BBMRI Negotiator?</t>
-  </si>
-  <si>
-    <t>Your current selection of biobanks along with your filtering criteria will be sent to the BBMRI Negotiator. Are you sure?</t>
-  </si>
-  <si>
-    <t>dataexplorer_directory_export_dialog_message</t>
-  </si>
-  <si>
-    <t>dataexplorer_directory_export_no_filters</t>
-  </si>
-  <si>
-    <t>Please filter the collections before sending a request to the negotiator.</t>
   </si>
 </sst>
 </file>
@@ -792,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -902,255 +866,206 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>84</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>28</v>
+      <c r="A23" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" t="s">
-        <v>40</v>
+        <v>52</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" t="s">
-        <v>41</v>
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>55</v>
+        <v>65</v>
+      </c>
+      <c r="B34" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
+      </c>
+      <c r="B35" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>61</v>
-      </c>
-      <c r="B38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" t="s">
-        <v>65</v>
-      </c>
-      <c r="B40" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="A43" t="s">
-        <v>71</v>
-      </c>
-      <c r="B43" t="s">
         <v>72</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>